<commit_message>
Datasets have been upgraded
Read full documentation in the pdf file.
</commit_message>
<xml_diff>
--- a/templates/MathDIY-datasets.xlsx
+++ b/templates/MathDIY-datasets.xlsx
@@ -37316,7 +37316,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve"> = Human Development Index (indexed with x</t>
+      <t xml:space="preserve"> = Human Development Index; indexed with x</t>
     </r>
   </si>
   <si>
@@ -37577,7 +37577,7 @@
         <color indexed="8"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
-      <t xml:space="preserve"> = Human Development Index (indexed with x</t>
+      <t xml:space="preserve"> = Human Development Index (indexed with x)</t>
     </r>
   </si>
   <si>
@@ -44969,10 +44969,10 @@
     <col min="1" max="1" width="8.32812" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.4297" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.5312" style="1" customWidth="1"/>
-    <col min="4" max="4" width="37.3516" style="1" customWidth="1"/>
+    <col min="4" max="4" width="38.2266" style="1" customWidth="1"/>
     <col min="5" max="5" width="37.4219" style="1" customWidth="1"/>
     <col min="6" max="8" width="13.5781" style="1" customWidth="1"/>
-    <col min="9" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
@@ -45727,7 +45727,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" ht="636.85" customHeight="1">
+    <row r="30" ht="622.5" customHeight="1">
       <c r="A30" t="s" s="7">
         <v>129</v>
       </c>
@@ -45753,7 +45753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" ht="1339.7" customHeight="1">
+    <row r="31" ht="1325.35" customHeight="1">
       <c r="A31" t="s" s="7">
         <v>135</v>
       </c>
@@ -45779,7 +45779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" ht="794.6" customHeight="1">
+    <row r="32" ht="751.6" customHeight="1">
       <c r="A32" t="s" s="7">
         <v>140</v>
       </c>
@@ -45805,7 +45805,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" ht="321.25" customHeight="1">
+    <row r="33" ht="306.95" customHeight="1">
       <c r="A33" t="s" s="7">
         <v>146</v>
       </c>
@@ -48353,7 +48353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" ht="249.55" customHeight="1">
+    <row r="131" ht="235.2" customHeight="1">
       <c r="A131" t="s" s="7">
         <v>540</v>
       </c>
@@ -48431,7 +48431,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" ht="220.85" customHeight="1">
+    <row r="134" ht="209.25" customHeight="1">
       <c r="A134" t="s" s="7">
         <v>552</v>
       </c>
@@ -48561,7 +48561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" ht="880.7" customHeight="1">
+    <row r="139" ht="837.65" customHeight="1">
       <c r="A139" t="s" s="7">
         <v>571</v>
       </c>
@@ -50641,7 +50641,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="219" ht="364.3" customHeight="1">
+    <row r="219" ht="349.95" customHeight="1">
       <c r="A219" t="s" s="7">
         <v>877</v>
       </c>
@@ -51239,7 +51239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="242" ht="450.35" customHeight="1">
+    <row r="242" ht="421.7" customHeight="1">
       <c r="A242" t="s" s="7">
         <v>976</v>
       </c>
@@ -51369,7 +51369,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="247" ht="579.6" customHeight="1">
+    <row r="247" ht="550.45" customHeight="1">
       <c r="A247" t="s" s="7">
         <v>1001</v>
       </c>
@@ -51421,7 +51421,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="249" ht="679.85" customHeight="1">
+    <row r="249" ht="665.55" customHeight="1">
       <c r="A249" t="s" s="7">
         <v>1011</v>
       </c>
@@ -51447,7 +51447,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="250" ht="837.65" customHeight="1">
+    <row r="250" ht="780.3" customHeight="1">
       <c r="A250" t="s" s="7">
         <v>1016</v>
       </c>
@@ -51473,7 +51473,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="251" ht="1311" customHeight="1">
+    <row r="251" ht="1267.95" customHeight="1">
       <c r="A251" t="s" s="7">
         <v>1021</v>
       </c>
@@ -51525,7 +51525,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="253" ht="637.35" customHeight="1">
+    <row r="253" ht="623" customHeight="1">
       <c r="A253" t="s" s="7">
         <v>1031</v>
       </c>

</xml_diff>